<commit_message>
Preliminary EDA, fixed null values
</commit_message>
<xml_diff>
--- a/Data/imaging_data.xlsx
+++ b/Data/imaging_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonahschwartz/Desktop/ENT Pre-Op Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonahschwartz/Documents/GitHub/Projects/ent-imaging-analysis/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACCD005F-5FB2-E04F-8A50-DD5EFDC6EB28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{323512C4-4E17-5A4B-9CCD-78C8DBF94931}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1640" yWindow="500" windowWidth="28800" windowHeight="16440" xr2:uid="{9C7DD11A-90AC-4141-B5D8-9465E75F7745}"/>
+    <workbookView xWindow="0" yWindow="1280" windowWidth="28800" windowHeight="16440" xr2:uid="{9C7DD11A-90AC-4141-B5D8-9465E75F7745}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3248" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3252" uniqueCount="49">
   <si>
     <t>Patient ID</t>
   </si>
@@ -586,8 +586,8 @@
   <dimension ref="A1:K406"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G18" sqref="G18"/>
+      <pane ySplit="1" topLeftCell="A223" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E226" sqref="E226"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2435,6 +2435,9 @@
       <c r="C53" s="2">
         <v>46</v>
       </c>
+      <c r="D53" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="E53" s="2" t="s">
         <v>18</v>
       </c>
@@ -2537,6 +2540,9 @@
       <c r="C56" s="2">
         <v>65</v>
       </c>
+      <c r="D56" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="E56" s="2" t="s">
         <v>47</v>
       </c>
@@ -4535,6 +4541,9 @@
       <c r="E113" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="F113" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="G113" s="2" t="s">
         <v>43</v>
       </c>
@@ -4630,6 +4639,9 @@
       </c>
       <c r="C116" s="2">
         <v>62</v>
+      </c>
+      <c r="D116" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="E116" s="2" t="s">
         <v>30</v>

</xml_diff>